<commit_message>
Updated webpage. add author page added, not yet working. Add discipline page added and working. homepage, pubish, javascrip and search.php are the pages that are up to date. the other pages need to be updated, all that needs to be done for that is including the publish.php page in the rest of the pages, a easy way to do this is just to copy the code from homepage.php and paste it on the outdated pages and then changing the tile and header to fit the name of each page.
</commit_message>
<xml_diff>
--- a/Work hours.xlsx
+++ b/Work hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">Time out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hours worked</t>
   </si>
 </sst>
 </file>
@@ -40,11 +43,12 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -66,6 +70,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,7 +128,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,6 +142,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,15 +166,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -171,6 +189,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -182,6 +203,9 @@
       <c r="C2" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -193,6 +217,9 @@
       <c r="C3" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -204,6 +231,9 @@
       <c r="C4" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -215,6 +245,9 @@
       <c r="C5" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -226,6 +259,9 @@
       <c r="C6" s="3" t="n">
         <v>0.875</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -237,6 +273,9 @@
       <c r="C7" s="3" t="n">
         <v>0.875</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -248,6 +287,9 @@
       <c r="C8" s="3" t="n">
         <v>0.875</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -259,6 +301,9 @@
       <c r="C9" s="3" t="n">
         <v>0.875</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -270,6 +315,9 @@
       <c r="C10" s="3" t="n">
         <v>0.875</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -281,6 +329,9 @@
       <c r="C11" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -292,6 +343,9 @@
       <c r="C12" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -303,6 +357,9 @@
       <c r="C13" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -314,6 +371,9 @@
       <c r="C14" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -325,6 +385,9 @@
       <c r="C15" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -336,6 +399,9 @@
       <c r="C16" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -346,6 +412,59 @@
       </c>
       <c r="C17" s="3" t="n">
         <v>0.458333333333333</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>43430</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>43437</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>43444</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>